<commit_message>
Agrega nuevas versiones de todos los diccionarios y esquemas
</commit_message>
<xml_diff>
--- a/DIEMSE to db.xlsx
+++ b/DIEMSE to db.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos_integracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos_integracion\27052023\archivos_integracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA0AC57-6441-48C0-A393-9D2820EF3C3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F8B60A-EE63-4095-8B59-D3CAF5451414}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" activeTab="4" xr2:uid="{37749BDB-DA12-497E-B3B5-A0FB37BA05F4}"/>
   </bookViews>
@@ -4478,7 +4478,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4552,6 +4552,10 @@
     <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4570,10 +4574,7 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5200,7 +5201,7 @@
   <dimension ref="A1:K376"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5886,7 +5887,7 @@
       <c r="J3" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="38" t="s">
         <v>1245</v>
       </c>
     </row>
@@ -5921,7 +5922,7 @@
       <c r="J4" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K4" s="37"/>
+      <c r="K4" s="39"/>
     </row>
     <row r="5" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -5954,7 +5955,7 @@
       <c r="J5" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -5987,7 +5988,7 @@
       <c r="J6" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K6" s="37"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -6020,7 +6021,7 @@
       <c r="J7" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K7" s="37"/>
+      <c r="K7" s="39"/>
     </row>
     <row r="8" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -6053,7 +6054,7 @@
       <c r="J8" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K8" s="37"/>
+      <c r="K8" s="39"/>
     </row>
     <row r="9" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -6086,7 +6087,7 @@
       <c r="J9" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K9" s="38"/>
+      <c r="K9" s="40"/>
     </row>
     <row r="10" spans="1:11" s="6" customFormat="1" ht="102.6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -6189,7 +6190,7 @@
       <c r="J12" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K12" s="33" t="s">
+      <c r="K12" s="35" t="s">
         <v>889</v>
       </c>
     </row>
@@ -6224,7 +6225,7 @@
       <c r="J13" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="36"/>
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -6257,7 +6258,7 @@
       <c r="J14" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K14" s="34"/>
+      <c r="K14" s="36"/>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -6290,7 +6291,7 @@
       <c r="J15" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K15" s="34"/>
+      <c r="K15" s="36"/>
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -6323,7 +6324,7 @@
       <c r="J16" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K16" s="35"/>
+      <c r="K16" s="37"/>
     </row>
     <row r="17" spans="1:11" s="6" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -29287,8 +29288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACF4232-7107-484C-B56C-5B13CEF154D2}">
   <dimension ref="A1:Q309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E207" sqref="E207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30120,7 +30121,7 @@
       <c r="G19" s="2">
         <v>0</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="H19" s="33" t="s">
         <v>632</v>
       </c>
       <c r="I19" s="10"/>
@@ -30163,7 +30164,7 @@
       <c r="G20" s="2">
         <v>0</v>
       </c>
-      <c r="H20" s="39" t="s">
+      <c r="H20" s="33" t="s">
         <v>633</v>
       </c>
       <c r="I20" s="10">
@@ -30208,7 +30209,7 @@
       <c r="G21" s="2">
         <v>0</v>
       </c>
-      <c r="H21" s="39" t="s">
+      <c r="H21" s="33" t="s">
         <v>886</v>
       </c>
       <c r="I21" s="10"/>
@@ -31160,7 +31161,7 @@
       <c r="G43" s="2">
         <v>0</v>
       </c>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="33" t="s">
         <v>653</v>
       </c>
       <c r="I43" s="10">
@@ -31205,7 +31206,7 @@
       <c r="G44" s="2">
         <v>0</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" s="33" t="s">
         <v>654</v>
       </c>
       <c r="I44" s="10">
@@ -31250,7 +31251,7 @@
       <c r="G45" s="2">
         <v>0</v>
       </c>
-      <c r="H45" s="39" t="s">
+      <c r="H45" s="33" t="s">
         <v>655</v>
       </c>
       <c r="I45" s="10"/>
@@ -31293,7 +31294,7 @@
       <c r="G46" s="2">
         <v>0</v>
       </c>
-      <c r="H46" s="39" t="s">
+      <c r="H46" s="33" t="s">
         <v>656</v>
       </c>
       <c r="I46" s="10"/>
@@ -31336,7 +31337,7 @@
       <c r="G47" s="2">
         <v>0</v>
       </c>
-      <c r="H47" s="39" t="s">
+      <c r="H47" s="33" t="s">
         <v>657</v>
       </c>
       <c r="I47" s="10">
@@ -32749,7 +32750,7 @@
         <v>991</v>
       </c>
       <c r="N79" s="2"/>
-      <c r="O79" s="40" t="s">
+      <c r="O79" s="34" t="s">
         <v>1261</v>
       </c>
       <c r="P79" s="2" t="s">
@@ -32796,7 +32797,7 @@
       <c r="L80" s="11"/>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
-      <c r="O80" s="40" t="s">
+      <c r="O80" s="34" t="s">
         <v>1261</v>
       </c>
       <c r="P80" s="2" t="s">
@@ -32841,7 +32842,7 @@
       <c r="L81" s="11"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
-      <c r="O81" s="40" t="s">
+      <c r="O81" s="34" t="s">
         <v>1261</v>
       </c>
       <c r="P81" s="2" t="s">
@@ -38548,9 +38549,9 @@
         <v>907</v>
       </c>
       <c r="G207" s="2">
-        <v>0</v>
-      </c>
-      <c r="H207" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H207" s="41" t="s">
         <v>798</v>
       </c>
       <c r="I207" s="10">
@@ -38638,7 +38639,7 @@
       <c r="G209" s="2">
         <v>0</v>
       </c>
-      <c r="H209" s="39" t="s">
+      <c r="H209" s="33" t="s">
         <v>886</v>
       </c>
       <c r="I209" s="10"/>
@@ -38681,7 +38682,7 @@
       <c r="G210" s="2">
         <v>0</v>
       </c>
-      <c r="H210" s="39" t="s">
+      <c r="H210" s="33" t="s">
         <v>800</v>
       </c>
       <c r="I210" s="10">
@@ -38726,7 +38727,7 @@
       <c r="G211" s="2">
         <v>0</v>
       </c>
-      <c r="H211" s="39" t="s">
+      <c r="H211" s="33" t="s">
         <v>801</v>
       </c>
       <c r="I211" s="10"/>

</xml_diff>

<commit_message>
Agrega nuevas versiones de DIEMSE, F63 y F81
</commit_message>
<xml_diff>
--- a/DIEMSE to db.xlsx
+++ b/DIEMSE to db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos_integracion\27052023\archivos_integracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F8B60A-EE63-4095-8B59-D3CAF5451414}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F415A11A-F7F4-45AA-BBBF-51014A4B229A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" activeTab="4" xr2:uid="{37749BDB-DA12-497E-B3B5-A0FB37BA05F4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17041" uniqueCount="1263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17041" uniqueCount="1264">
   <si>
     <t>Nombre de la Entidad</t>
   </si>
@@ -3856,6 +3856,9 @@
   </si>
   <si>
     <t>Nombre del atributo</t>
+  </si>
+  <si>
+    <t>D_DEC_TCIOPMO1(003)</t>
   </si>
 </sst>
 </file>
@@ -4556,6 +4559,7 @@
     <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4574,7 +4578,6 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5887,7 +5890,7 @@
       <c r="J3" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="39" t="s">
         <v>1245</v>
       </c>
     </row>
@@ -5922,7 +5925,7 @@
       <c r="J4" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K4" s="39"/>
+      <c r="K4" s="40"/>
     </row>
     <row r="5" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -5955,7 +5958,7 @@
       <c r="J5" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K5" s="39"/>
+      <c r="K5" s="40"/>
     </row>
     <row r="6" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -5988,7 +5991,7 @@
       <c r="J6" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K6" s="39"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -6021,7 +6024,7 @@
       <c r="J7" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K7" s="39"/>
+      <c r="K7" s="40"/>
     </row>
     <row r="8" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -6054,7 +6057,7 @@
       <c r="J8" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K8" s="39"/>
+      <c r="K8" s="40"/>
     </row>
     <row r="9" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -6087,7 +6090,7 @@
       <c r="J9" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K9" s="40"/>
+      <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" s="6" customFormat="1" ht="102.6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -6190,7 +6193,7 @@
       <c r="J12" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K12" s="35" t="s">
+      <c r="K12" s="36" t="s">
         <v>889</v>
       </c>
     </row>
@@ -6225,7 +6228,7 @@
       <c r="J13" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -6258,7 +6261,7 @@
       <c r="J14" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K14" s="36"/>
+      <c r="K14" s="37"/>
     </row>
     <row r="15" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -6291,7 +6294,7 @@
       <c r="J15" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K15" s="36"/>
+      <c r="K15" s="37"/>
     </row>
     <row r="16" spans="1:11" s="6" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -6324,7 +6327,7 @@
       <c r="J16" s="10" t="s">
         <v>1227</v>
       </c>
-      <c r="K16" s="37"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:11" s="6" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -29288,8 +29291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACF4232-7107-484C-B56C-5B13CEF154D2}">
   <dimension ref="A1:Q309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E207" sqref="E207"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O79" sqref="O79:O81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32798,7 +32801,7 @@
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="34" t="s">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="P80" s="2" t="s">
         <v>995</v>
@@ -32843,7 +32846,7 @@
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="34" t="s">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="P81" s="2" t="s">
         <v>997</v>
@@ -38551,7 +38554,7 @@
       <c r="G207" s="2">
         <v>1</v>
       </c>
-      <c r="H207" s="41" t="s">
+      <c r="H207" s="35" t="s">
         <v>798</v>
       </c>
       <c r="I207" s="10">

</xml_diff>

<commit_message>
Agrega modificaciones en ddl y genera esquemas DIEMSE
</commit_message>
<xml_diff>
--- a/DIEMSE to db.xlsx
+++ b/DIEMSE to db.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos_integracion\27052023\archivos_integracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos_integracion\27052023\archivos_integracion\28052024\archivos_integracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F415A11A-F7F4-45AA-BBBF-51014A4B229A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7B219C-CFE3-44C5-A846-341E1600DD75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" activeTab="4" xr2:uid="{37749BDB-DA12-497E-B3B5-A0FB37BA05F4}"/>
   </bookViews>
@@ -29291,8 +29291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACF4232-7107-484C-B56C-5B13CEF154D2}">
   <dimension ref="A1:Q309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O79" sqref="O79:O81"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M229" sqref="M229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39376,7 +39376,7 @@
       </c>
       <c r="L225" s="11"/>
       <c r="M225" s="2" t="s">
-        <v>1224</v>
+        <v>1164</v>
       </c>
       <c r="N225" s="2"/>
       <c r="O225" s="9"/>

</xml_diff>

<commit_message>
Agrega nuevas versiones de DIEMSE y F76
</commit_message>
<xml_diff>
--- a/DIEMSE to db.xlsx
+++ b/DIEMSE to db.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos_integracion\27052023\archivos_integracion\28052024\archivos_integracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos_integracion\27052023\archivos_integracion\28052024\archivos_integracion\archivos_integracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7B219C-CFE3-44C5-A846-341E1600DD75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF69D9C-25EF-46CA-B0CB-5F0D82032CF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" activeTab="4" xr2:uid="{37749BDB-DA12-497E-B3B5-A0FB37BA05F4}"/>
   </bookViews>
@@ -4481,7 +4481,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4577,6 +4577,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -22481,8 +22484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1CEA37-802E-481C-BEE1-E2710E02EE1D}">
   <dimension ref="A1:F376"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="F221" sqref="F221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29291,8 +29294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACF4232-7107-484C-B56C-5B13CEF154D2}">
   <dimension ref="A1:Q309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M229" sqref="M229"/>
+    <sheetView tabSelected="1" topLeftCell="A198" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E213" sqref="E213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38816,7 +38819,7 @@
       <c r="G213" s="15">
         <v>0</v>
       </c>
-      <c r="H213" s="3" t="s">
+      <c r="H213" s="13" t="s">
         <v>803</v>
       </c>
       <c r="I213" s="10">
@@ -38825,8 +38828,8 @@
       <c r="J213" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="K213" s="11">
-        <v>1</v>
+      <c r="K213" s="42">
+        <v>5</v>
       </c>
       <c r="L213" s="11"/>
       <c r="M213" s="2"/>

</xml_diff>